<commit_message>
Corrección nombre subsección escaleta
Corrección nombre sección 2.3.3
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion03/Escaleta_CN_08_03_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion03/Escaleta_CN_08_03_CO.xlsx
@@ -18,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$25</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="218">
   <si>
     <t>Asignatura</t>
   </si>
@@ -392,9 +392,6 @@
     <t>m102AB</t>
   </si>
   <si>
-    <t>CN_08_02_CO</t>
-  </si>
-  <si>
     <t>Consolidación</t>
   </si>
   <si>
@@ -518,9 +515,6 @@
     <t>Menú principal con las opciones "Innata" y "adquirida". La opción Innata no se divide más, y al entrra se habla de que depende de los leucocitos o glóbulos blancos, recordando brevemente o mencionando los tipos que hay (fagocitos, células NK, etc), dado que esto ya se expuso. También se menciona la respuesta inflamatoria y la fiebre, también recordando que ya se expuso. La opción Adquirida tiene las opciones de "natural" o articial", y dentro de cada opción se explican mencionando que depende de los linfocitos de memoria (linfocitos B y T de memoria), y a continiacuión que pueden ser inmunidad activa o pasiva (aplica tanto para natural como adquirida), explicando qué es cada una.</t>
   </si>
   <si>
-    <t>Las vacunas y el suero inmunológico</t>
-  </si>
-  <si>
     <t>Responde sobre la inmunización activa y pasiva</t>
   </si>
   <si>
@@ -681,6 +675,9 @@
   </si>
   <si>
     <t>Recurso M101A-03</t>
+  </si>
+  <si>
+    <t>Las vacunas</t>
   </si>
 </sst>
 </file>
@@ -892,16 +889,34 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -941,24 +956,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1267,9 +1264,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,112 +1294,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="22" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="J1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="35" t="s">
+      <c r="K1" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="L1" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="39"/>
-      <c r="O1" s="27" t="s">
+      <c r="N1" s="45"/>
+      <c r="O1" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="P1" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="42" t="s">
+      <c r="Q1" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="46" t="s">
+      <c r="R1" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="42" t="s">
+      <c r="S1" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="44" t="s">
+      <c r="T1" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="42" t="s">
+      <c r="U1" s="27" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="22" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="34"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="40"/>
       <c r="M2" s="23" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="47"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="45"/>
-      <c r="U2" s="43"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="28"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>133</v>
-      </c>
       <c r="D3" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="9"/>
       <c r="G3" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H3" s="9">
         <v>1</v>
@@ -1411,7 +1408,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>20</v>
@@ -1424,7 +1421,7 @@
       </c>
       <c r="N3" s="8"/>
       <c r="O3" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>19</v>
@@ -1433,16 +1430,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="S3" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="T3" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="S3" s="19" t="s">
+      <c r="U3" s="19" t="s">
         <v>203</v>
-      </c>
-      <c r="T3" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="U3" s="19" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1450,20 +1447,20 @@
         <v>17</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H4" s="9">
         <v>2</v>
@@ -1472,7 +1469,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>20</v>
@@ -1485,7 +1482,7 @@
         <v>43</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>19</v>
@@ -1494,16 +1491,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="S4" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="S4" s="19" t="s">
-        <v>128</v>
-      </c>
       <c r="T4" s="21" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="U4" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1511,20 +1508,20 @@
         <v>17</v>
       </c>
       <c r="B5" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>122</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>123</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H5" s="9">
         <v>3</v>
@@ -1533,7 +1530,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>20</v>
@@ -1546,7 +1543,7 @@
         <v>52</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P5" s="9" t="s">
         <v>19</v>
@@ -1555,16 +1552,16 @@
         <v>6</v>
       </c>
       <c r="R5" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="S5" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="S5" s="10" t="s">
-        <v>128</v>
-      </c>
       <c r="T5" s="12" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="U5" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1572,18 +1569,18 @@
         <v>17</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="9"/>
       <c r="G6" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H6" s="9">
         <v>4</v>
@@ -1592,7 +1589,7 @@
         <v>19</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>20</v>
@@ -1605,7 +1602,7 @@
       </c>
       <c r="N6" s="8"/>
       <c r="O6" s="9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>19</v>
@@ -1614,16 +1611,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="S6" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="T6" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="U6" s="10" t="s">
         <v>203</v>
-      </c>
-      <c r="T6" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="U6" s="10" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1631,20 +1628,20 @@
         <v>17</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H7" s="9">
         <v>5</v>
@@ -1653,7 +1650,7 @@
         <v>19</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>19</v>
@@ -1668,19 +1665,19 @@
         <v>19</v>
       </c>
       <c r="Q7" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="R7" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="S7" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="R7" s="11" t="s">
+      <c r="T7" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="U7" s="10" t="s">
         <v>191</v>
-      </c>
-      <c r="S7" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="T7" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="U7" s="10" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1688,20 +1685,20 @@
         <v>17</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H8" s="9">
         <v>6</v>
@@ -1710,7 +1707,7 @@
         <v>19</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>20</v>
@@ -1723,7 +1720,7 @@
         <v>32</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="P8" s="9" t="s">
         <v>20</v>
@@ -1732,16 +1729,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="S8" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="S8" s="10" t="s">
+      <c r="T8" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="T8" s="12" t="s">
+      <c r="U8" s="10" t="s">
         <v>129</v>
-      </c>
-      <c r="U8" s="10" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1749,20 +1746,20 @@
         <v>17</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H9" s="9">
         <v>7</v>
@@ -1771,7 +1768,7 @@
         <v>19</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>19</v>
@@ -1786,19 +1783,19 @@
         <v>19</v>
       </c>
       <c r="Q9" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="R9" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="S9" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="R9" s="11" t="s">
+      <c r="T9" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="U9" s="10" t="s">
         <v>191</v>
-      </c>
-      <c r="S9" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="T9" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="U9" s="10" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1806,20 +1803,20 @@
         <v>17</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H10" s="9">
         <v>8</v>
@@ -1828,7 +1825,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>20</v>
@@ -1841,7 +1838,7 @@
         <v>23</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="P10" s="9" t="s">
         <v>19</v>
@@ -1850,16 +1847,16 @@
         <v>6</v>
       </c>
       <c r="R10" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="S10" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="S10" s="10" t="s">
-        <v>128</v>
-      </c>
       <c r="T10" s="12" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="U10" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1867,20 +1864,20 @@
         <v>17</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H11" s="9">
         <v>9</v>
@@ -1889,7 +1886,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>19</v>
@@ -1904,19 +1901,19 @@
         <v>19</v>
       </c>
       <c r="Q11" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="R11" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="S11" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="R11" s="11" t="s">
+      <c r="T11" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="U11" s="10" t="s">
         <v>191</v>
-      </c>
-      <c r="S11" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="T11" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="U11" s="10" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1924,20 +1921,20 @@
         <v>17</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H12" s="9">
         <v>10</v>
@@ -1946,7 +1943,7 @@
         <v>19</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>20</v>
@@ -1959,7 +1956,7 @@
       </c>
       <c r="N12" s="8"/>
       <c r="O12" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P12" s="9" t="s">
         <v>19</v>
@@ -1968,16 +1965,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="S12" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="T12" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="U12" s="10" t="s">
         <v>203</v>
-      </c>
-      <c r="T12" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="U12" s="10" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1985,22 +1982,22 @@
         <v>17</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>164</v>
+        <v>217</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H13" s="9">
         <v>11</v>
@@ -2009,7 +2006,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>20</v>
@@ -2022,7 +2019,7 @@
         <v>43</v>
       </c>
       <c r="O13" s="9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="P13" s="9" t="s">
         <v>19</v>
@@ -2031,16 +2028,16 @@
         <v>6</v>
       </c>
       <c r="R13" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="S13" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="S13" s="10" t="s">
-        <v>128</v>
-      </c>
       <c r="T13" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="U13" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2048,22 +2045,22 @@
         <v>17</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>164</v>
+        <v>217</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H14" s="9">
         <v>12</v>
@@ -2072,7 +2069,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>19</v>
@@ -2087,19 +2084,19 @@
         <v>20</v>
       </c>
       <c r="Q14" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="R14" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="S14" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="R14" s="11" t="s">
+      <c r="T14" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="U14" s="10" t="s">
         <v>191</v>
-      </c>
-      <c r="S14" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="T14" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="U14" s="10" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2107,20 +2104,20 @@
         <v>17</v>
       </c>
       <c r="B15" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="E15" s="13" t="s">
         <v>122</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>123</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H15" s="9">
         <v>13</v>
@@ -2129,7 +2126,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>20</v>
@@ -2149,16 +2146,16 @@
         <v>6</v>
       </c>
       <c r="R15" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="S15" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="S15" s="10" t="s">
-        <v>128</v>
-      </c>
       <c r="T15" s="12" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="U15" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2166,18 +2163,18 @@
         <v>17</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="9"/>
       <c r="G16" s="16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H16" s="9">
         <v>15</v>
@@ -2186,7 +2183,7 @@
         <v>19</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>20</v>
@@ -2199,7 +2196,7 @@
       </c>
       <c r="N16" s="8"/>
       <c r="O16" s="9" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="P16" s="9" t="s">
         <v>19</v>
@@ -2208,16 +2205,16 @@
         <v>6</v>
       </c>
       <c r="R16" s="11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="S16" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="T16" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="U16" s="10" t="s">
         <v>203</v>
-      </c>
-      <c r="T16" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="U16" s="10" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2225,16 +2222,16 @@
         <v>17</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="13"/>
       <c r="F17" s="9"/>
       <c r="G17" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H17" s="9">
         <v>16</v>
@@ -2243,7 +2240,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>20</v>
@@ -2256,7 +2253,7 @@
         <v>120</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="P17" s="9" t="s">
         <v>19</v>
@@ -2265,16 +2262,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="S17" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="S17" s="10" t="s">
-        <v>128</v>
-      </c>
       <c r="T17" s="12" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="U17" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2282,16 +2279,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="13"/>
       <c r="F18" s="9"/>
       <c r="G18" s="16" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H18" s="9">
         <v>17</v>
@@ -2300,7 +2297,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>20</v>
@@ -2313,7 +2310,7 @@
         <v>28</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="P18" s="9" t="s">
         <v>19</v>
@@ -2322,16 +2319,16 @@
         <v>6</v>
       </c>
       <c r="R18" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="S18" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="S18" s="10" t="s">
-        <v>128</v>
-      </c>
       <c r="T18" s="12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="U18" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2339,18 +2336,18 @@
         <v>17</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H19" s="9">
         <v>18</v>
@@ -2359,7 +2356,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>20</v>
@@ -2379,16 +2376,16 @@
         <v>6</v>
       </c>
       <c r="R19" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="S19" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="S19" s="10" t="s">
-        <v>128</v>
-      </c>
       <c r="T19" s="12" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="U19" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2396,18 +2393,18 @@
         <v>17</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E20" s="13"/>
       <c r="F20" s="9"/>
       <c r="G20" s="16" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H20" s="9">
         <v>19</v>
@@ -2416,7 +2413,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>19</v>
@@ -2431,19 +2428,19 @@
         <v>19</v>
       </c>
       <c r="Q20" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="R20" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="S20" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="R20" s="11" t="s">
+      <c r="T20" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="U20" s="10" t="s">
         <v>191</v>
-      </c>
-      <c r="S20" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="T20" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="U20" s="10" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2451,18 +2448,18 @@
         <v>17</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="9"/>
       <c r="G21" s="16" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H21" s="9">
         <v>20</v>
@@ -2471,7 +2468,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>19</v>
@@ -2486,19 +2483,19 @@
         <v>19</v>
       </c>
       <c r="Q21" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="R21" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="S21" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="R21" s="11" t="s">
+      <c r="T21" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="U21" s="10" t="s">
         <v>191</v>
-      </c>
-      <c r="S21" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="T21" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="U21" s="10" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2506,18 +2503,18 @@
         <v>17</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="9"/>
       <c r="G22" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H22" s="9">
         <v>21</v>
@@ -2526,7 +2523,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>19</v>
@@ -2541,19 +2538,19 @@
         <v>19</v>
       </c>
       <c r="Q22" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="R22" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="S22" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="R22" s="11" t="s">
+      <c r="T22" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="U22" s="10" t="s">
         <v>191</v>
-      </c>
-      <c r="S22" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="T22" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="U22" s="10" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2561,13 +2558,13 @@
         <v>17</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E23" s="13"/>
       <c r="F23" s="9"/>
@@ -2581,7 +2578,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>20</v>
@@ -2606,18 +2603,18 @@
         <v>17</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E24" s="13"/>
       <c r="F24" s="9"/>
       <c r="G24" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H24" s="9">
         <v>23</v>
@@ -2626,7 +2623,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>20</v>
@@ -2646,16 +2643,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="S24" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="S24" s="10" t="s">
+      <c r="T24" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="T24" s="12" t="s">
+      <c r="U24" s="10" t="s">
         <v>129</v>
-      </c>
-      <c r="U24" s="10" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2663,18 +2660,18 @@
         <v>17</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E25" s="13"/>
       <c r="F25" s="9"/>
       <c r="G25" s="16" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H25" s="9">
         <v>24</v>
@@ -2683,7 +2680,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K25" s="7" t="s">
         <v>20</v>
@@ -2703,16 +2700,16 @@
         <v>6</v>
       </c>
       <c r="R25" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="S25" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="S25" s="10" t="s">
-        <v>128</v>
-      </c>
       <c r="T25" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="U25" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3888,378 +3885,372 @@
       <c r="T76" s="12"/>
       <c r="U76" s="10"/>
     </row>
-    <row r="78" spans="1:21" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="79" spans="1:21" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="80" spans="1:21" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="81" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="82" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="83" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="84" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="85" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="86" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="87" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="88" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="89" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="90" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="91" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="98" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="99" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="100" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="101" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="102" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="103" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="104" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="105" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="106" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="107" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="108" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="109" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="110" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="111" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="112" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="113" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="114" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="115" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="116" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="117" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="118" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="119" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="120" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="121" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="122" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="123" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="124" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="125" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="126" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="127" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="128" spans="1:1" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="129" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="130" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="131" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="132" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="133" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="134" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="135" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="136" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="137" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="138" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="139" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="140" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="141" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="142" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="143" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="144" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="145" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="146" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="147" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="148" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="149" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="150" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="151" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="152" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="153" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="154" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="155" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="156" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="157" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="158" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="159" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="160" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="161" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="162" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="163" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="164" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="165" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="166" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="167" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="168" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="169" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="170" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="171" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="172" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="173" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="174" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="175" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="176" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="177" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="178" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="179" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="180" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="181" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="182" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="183" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="184" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="185" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="186" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="187" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="188" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="189" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="190" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="191" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="192" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="193" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="194" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="195" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="196" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="197" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="198" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="199" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="200" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="201" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="202" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="203" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="204" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="205" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="206" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="207" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="208" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="209" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="210" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="211" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="212" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="213" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="214" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="215" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="216" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="217" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="218" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="219" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="220" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="221" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="222" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="223" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="224" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="225" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="226" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="227" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="228" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="229" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="230" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="231" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="232" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="233" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="234" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="235" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="236" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="237" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="238" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="239" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="240" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="241" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="242" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="243" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="244" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="245" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="246" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="247" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="248" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="249" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="250" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="251" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="252" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="253" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="254" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="255" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="256" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="257" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="258" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="259" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="260" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="261" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="262" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="263" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="264" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="265" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="266" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="267" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="268" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="269" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="270" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="271" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="272" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="273" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="274" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="275" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="276" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="277" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="278" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="279" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="280" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="281" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="282" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="283" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="284" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="285" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="286" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="287" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="288" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="289" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="290" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="129" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="130" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="131" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="132" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="133" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="134" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="135" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="136" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="137" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="138" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="139" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="140" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="141" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="142" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="143" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="144" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="145" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="146" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="147" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="148" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="149" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="150" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="151" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="152" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="153" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="154" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="155" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="156" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="157" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="158" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="159" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="160" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="161" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="162" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="163" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="164" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="165" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="166" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="167" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="168" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="169" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="170" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="171" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="172" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="173" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="174" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="175" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="176" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="177" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="178" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="179" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="180" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="181" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="182" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="183" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="184" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="185" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="186" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="187" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="188" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="189" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="190" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="191" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="192" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="193" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="194" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="195" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="196" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="197" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="198" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="199" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="200" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="201" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="202" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="203" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="204" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="205" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="206" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="207" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="208" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="209" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="210" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="211" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="212" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="213" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="214" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="215" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="216" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="217" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="218" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="219" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="220" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="221" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="222" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="223" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="224" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="225" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="226" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="227" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="228" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="229" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="230" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="231" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="232" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="233" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="234" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="235" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="236" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="237" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="238" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="239" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="240" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="241" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="242" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="243" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="244" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="245" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="246" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="247" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="248" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="249" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="250" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="251" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="252" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="253" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="254" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="255" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="256" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="257" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="258" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="259" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="260" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="261" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="262" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="263" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="264" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="265" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="266" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="267" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="268" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="269" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="270" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="271" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="272" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="273" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="274" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="275" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="276" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="277" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="278" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="279" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="280" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="281" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="282" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="283" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="284" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="285" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="286" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="287" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="288" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="289" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="290" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A1:U25">
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4274,6 +4265,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4361,7 +4358,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -4404,7 +4401,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -4423,7 +4420,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
@@ -4439,7 +4436,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
@@ -4473,7 +4470,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -4488,7 +4485,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>

</xml_diff>

<commit_message>
Correcciones manuscrito y escaletas.
Correcciones de estilo.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion03/Escaleta_CN_08_03_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion03/Escaleta_CN_08_03_CO.xlsx
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$25</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -428,9 +428,6 @@
     <t>Tres menús: defensas externas (piel, pelo, etc.), defensas internas inespecíficas (ácidos, fiebre, inflamación, etc.), y barreras internas específicas (generalidades del sistema inmune. Muy sencillo).</t>
   </si>
   <si>
-    <t>Mecanismos de defensa ante los patógenos</t>
-  </si>
-  <si>
     <t>Actividad acerca de las defensas internas y externas contra patógenos</t>
   </si>
   <si>
@@ -545,9 +542,6 @@
     <t>Actividad acerca de las enfermedades relacionadas con el sistema inmunitario</t>
   </si>
   <si>
-    <t>Enfermedades relacionadas con el sistema inmunitario</t>
-  </si>
-  <si>
     <t>El sistema inmunitario y la donación de tejidos</t>
   </si>
   <si>
@@ -678,6 +672,12 @@
   </si>
   <si>
     <t>Las vacunas</t>
+  </si>
+  <si>
+    <t>Los mecanismos de defensa ante los patógenos</t>
+  </si>
+  <si>
+    <t>Las enfermedades relacionadas con el sistema inmunitario</t>
   </si>
 </sst>
 </file>
@@ -1264,9 +1264,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U290"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1394,12 +1394,12 @@
         <v>132</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="9"/>
       <c r="G3" s="16" t="s">
-        <v>134</v>
+        <v>216</v>
       </c>
       <c r="H3" s="9">
         <v>1</v>
@@ -1408,7 +1408,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>20</v>
@@ -1430,16 +1430,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="S3" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="T3" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="S3" s="19" t="s">
+      <c r="U3" s="19" t="s">
         <v>201</v>
-      </c>
-      <c r="T3" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="U3" s="19" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1453,14 +1453,14 @@
         <v>132</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H4" s="9">
         <v>2</v>
@@ -1469,7 +1469,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>20</v>
@@ -1482,7 +1482,7 @@
         <v>43</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>19</v>
@@ -1497,7 +1497,7 @@
         <v>127</v>
       </c>
       <c r="T4" s="21" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="U4" s="19" t="s">
         <v>129</v>
@@ -1514,14 +1514,14 @@
         <v>132</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>122</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H5" s="9">
         <v>3</v>
@@ -1530,7 +1530,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>20</v>
@@ -1543,7 +1543,7 @@
         <v>52</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P5" s="9" t="s">
         <v>19</v>
@@ -1558,7 +1558,7 @@
         <v>127</v>
       </c>
       <c r="T5" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="U5" s="10" t="s">
         <v>129</v>
@@ -1575,12 +1575,12 @@
         <v>132</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="9"/>
       <c r="G6" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H6" s="9">
         <v>4</v>
@@ -1589,7 +1589,7 @@
         <v>19</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>20</v>
@@ -1602,7 +1602,7 @@
       </c>
       <c r="N6" s="8"/>
       <c r="O6" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>19</v>
@@ -1611,16 +1611,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="S6" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="T6" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="U6" s="10" t="s">
         <v>201</v>
-      </c>
-      <c r="T6" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="U6" s="10" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1634,14 +1634,14 @@
         <v>132</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H7" s="9">
         <v>5</v>
@@ -1650,7 +1650,7 @@
         <v>19</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>19</v>
@@ -1665,19 +1665,19 @@
         <v>19</v>
       </c>
       <c r="Q7" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="R7" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="S7" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="R7" s="11" t="s">
+      <c r="T7" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="U7" s="10" t="s">
         <v>189</v>
-      </c>
-      <c r="S7" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="T7" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="U7" s="10" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1691,23 +1691,23 @@
         <v>132</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H8" s="9">
         <v>6</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>20</v>
@@ -1720,7 +1720,7 @@
         <v>32</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="P8" s="9" t="s">
         <v>20</v>
@@ -1752,14 +1752,14 @@
         <v>132</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H9" s="9">
         <v>7</v>
@@ -1768,7 +1768,7 @@
         <v>19</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>19</v>
@@ -1783,19 +1783,19 @@
         <v>19</v>
       </c>
       <c r="Q9" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="R9" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="S9" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="R9" s="11" t="s">
+      <c r="T9" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="U9" s="10" t="s">
         <v>189</v>
-      </c>
-      <c r="S9" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="T9" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="U9" s="10" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1809,14 +1809,14 @@
         <v>132</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H10" s="9">
         <v>8</v>
@@ -1825,7 +1825,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>20</v>
@@ -1838,7 +1838,7 @@
         <v>23</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P10" s="9" t="s">
         <v>19</v>
@@ -1853,7 +1853,7 @@
         <v>127</v>
       </c>
       <c r="T10" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="U10" s="10" t="s">
         <v>129</v>
@@ -1870,14 +1870,14 @@
         <v>132</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H11" s="9">
         <v>9</v>
@@ -1886,7 +1886,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>19</v>
@@ -1901,19 +1901,19 @@
         <v>19</v>
       </c>
       <c r="Q11" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="R11" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="S11" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="R11" s="11" t="s">
+      <c r="T11" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="U11" s="10" t="s">
         <v>189</v>
-      </c>
-      <c r="S11" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="T11" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="U11" s="10" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1927,14 +1927,14 @@
         <v>132</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H12" s="9">
         <v>10</v>
@@ -1943,7 +1943,7 @@
         <v>19</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>20</v>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="N12" s="8"/>
       <c r="O12" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P12" s="9" t="s">
         <v>19</v>
@@ -1965,16 +1965,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="S12" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="T12" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="U12" s="10" t="s">
         <v>201</v>
-      </c>
-      <c r="T12" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="U12" s="10" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1988,16 +1988,16 @@
         <v>132</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H13" s="9">
         <v>11</v>
@@ -2006,7 +2006,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>20</v>
@@ -2019,7 +2019,7 @@
         <v>43</v>
       </c>
       <c r="O13" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="P13" s="9" t="s">
         <v>19</v>
@@ -2034,7 +2034,7 @@
         <v>127</v>
       </c>
       <c r="T13" s="12" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="U13" s="10" t="s">
         <v>129</v>
@@ -2051,16 +2051,16 @@
         <v>132</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H14" s="9">
         <v>12</v>
@@ -2069,7 +2069,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>19</v>
@@ -2084,19 +2084,19 @@
         <v>20</v>
       </c>
       <c r="Q14" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="R14" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="S14" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="R14" s="11" t="s">
+      <c r="T14" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="U14" s="10" t="s">
         <v>189</v>
-      </c>
-      <c r="S14" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="T14" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="U14" s="10" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2110,14 +2110,14 @@
         <v>132</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>122</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H15" s="9">
         <v>13</v>
@@ -2126,7 +2126,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>20</v>
@@ -2152,7 +2152,7 @@
         <v>127</v>
       </c>
       <c r="T15" s="12" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="U15" s="10" t="s">
         <v>129</v>
@@ -2169,12 +2169,12 @@
         <v>132</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="9"/>
       <c r="G16" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H16" s="9">
         <v>15</v>
@@ -2183,7 +2183,7 @@
         <v>19</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>20</v>
@@ -2196,7 +2196,7 @@
       </c>
       <c r="N16" s="8"/>
       <c r="O16" s="9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="P16" s="9" t="s">
         <v>19</v>
@@ -2205,16 +2205,16 @@
         <v>6</v>
       </c>
       <c r="R16" s="11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="S16" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="T16" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="U16" s="10" t="s">
         <v>201</v>
-      </c>
-      <c r="T16" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="U16" s="10" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2231,7 +2231,7 @@
       <c r="E17" s="13"/>
       <c r="F17" s="9"/>
       <c r="G17" s="16" t="s">
-        <v>173</v>
+        <v>217</v>
       </c>
       <c r="H17" s="9">
         <v>16</v>
@@ -2240,7 +2240,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>20</v>
@@ -2253,7 +2253,7 @@
         <v>120</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="P17" s="9" t="s">
         <v>19</v>
@@ -2268,7 +2268,7 @@
         <v>127</v>
       </c>
       <c r="T17" s="12" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="U17" s="10" t="s">
         <v>129</v>
@@ -2288,7 +2288,7 @@
       <c r="E18" s="13"/>
       <c r="F18" s="9"/>
       <c r="G18" s="16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H18" s="9">
         <v>17</v>
@@ -2297,7 +2297,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>20</v>
@@ -2310,7 +2310,7 @@
         <v>28</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="P18" s="9" t="s">
         <v>19</v>
@@ -2325,7 +2325,7 @@
         <v>127</v>
       </c>
       <c r="T18" s="12" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="U18" s="10" t="s">
         <v>129</v>
@@ -2347,7 +2347,7 @@
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H19" s="9">
         <v>18</v>
@@ -2356,7 +2356,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>20</v>
@@ -2382,7 +2382,7 @@
         <v>127</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="U19" s="10" t="s">
         <v>129</v>
@@ -2404,7 +2404,7 @@
       <c r="E20" s="13"/>
       <c r="F20" s="9"/>
       <c r="G20" s="16" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H20" s="9">
         <v>19</v>
@@ -2413,7 +2413,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>19</v>
@@ -2428,19 +2428,19 @@
         <v>19</v>
       </c>
       <c r="Q20" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="R20" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="S20" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="R20" s="11" t="s">
+      <c r="T20" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="U20" s="10" t="s">
         <v>189</v>
-      </c>
-      <c r="S20" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="T20" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="U20" s="10" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2459,7 +2459,7 @@
       <c r="E21" s="13"/>
       <c r="F21" s="9"/>
       <c r="G21" s="16" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H21" s="9">
         <v>20</v>
@@ -2468,7 +2468,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>19</v>
@@ -2483,19 +2483,19 @@
         <v>19</v>
       </c>
       <c r="Q21" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="R21" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="S21" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="R21" s="11" t="s">
+      <c r="T21" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="U21" s="10" t="s">
         <v>189</v>
-      </c>
-      <c r="S21" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="T21" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="U21" s="10" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2514,7 +2514,7 @@
       <c r="E22" s="13"/>
       <c r="F22" s="9"/>
       <c r="G22" s="16" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H22" s="9">
         <v>21</v>
@@ -2523,7 +2523,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>19</v>
@@ -2538,19 +2538,19 @@
         <v>19</v>
       </c>
       <c r="Q22" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="R22" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="S22" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="R22" s="11" t="s">
+      <c r="T22" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="U22" s="10" t="s">
         <v>189</v>
-      </c>
-      <c r="S22" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="T22" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="U22" s="10" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2578,7 +2578,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>20</v>
@@ -2623,7 +2623,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>20</v>
@@ -2671,7 +2671,7 @@
       <c r="E25" s="13"/>
       <c r="F25" s="9"/>
       <c r="G25" s="16" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H25" s="9">
         <v>24</v>
@@ -2680,7 +2680,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="K25" s="7" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Correcciones CE y escaleta
Había un nombre de recurso repetido
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion03/Escaleta_CN_08_03_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion03/Escaleta_CN_08_03_CO.xlsx
@@ -16,14 +16,14 @@
     <sheet name="DATOS" sheetId="1" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$26</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="223">
   <si>
     <t>Asignatura</t>
   </si>
@@ -443,18 +443,9 @@
     <t>Los componentes del sistema inmunitario</t>
   </si>
   <si>
-    <t>Interactivo acerca del sistema inmunitario, que explica el sistema linfático y los tipos de glóbulos blancos</t>
-  </si>
-  <si>
-    <t>Interactivo que explica las defensas internas y externas de los organismos ante los patógenos</t>
-  </si>
-  <si>
     <t>El sistema linfático</t>
   </si>
   <si>
-    <t>Animación que explica la estructura y función del sistema linfático</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: Las defensas internas y externas</t>
   </si>
   <si>
@@ -473,15 +464,9 @@
     <t>Los glóbulos blancos y el sistema inmunitario</t>
   </si>
   <si>
-    <t>Interactivo con animación que muestra la función de los diferentes glóbulos blancos</t>
-  </si>
-  <si>
     <t>Los diferentes tipos de glóbulos blancos</t>
   </si>
   <si>
-    <t xml:space="preserve">Actividad acerca de los distintos tipos de glóbulos blancos y sus funciones </t>
-  </si>
-  <si>
     <t>Las palabras son tipos de glóbulos blancos, y las frases describen su función o características</t>
   </si>
   <si>
@@ -494,9 +479,6 @@
     <t>La relación entre el sistema linfático y el inmunitario</t>
   </si>
   <si>
-    <t>Actividad que pone a prueba los conocimientos acerca del sistema linfático</t>
-  </si>
-  <si>
     <t>No limitar las preguntas a los animales. Preguntar por la fiebre y la tendencia de la gente a combatirla apenas aparece.</t>
   </si>
   <si>
@@ -506,51 +488,24 @@
     <t>La inmunidad</t>
   </si>
   <si>
-    <t>Interactivo que explica qué es la inmunidad, tanto innata como adquirida</t>
-  </si>
-  <si>
-    <t>Menú principal con las opciones "Innata" y "adquirida". La opción Innata no se divide más, y al entrra se habla de que depende de los leucocitos o glóbulos blancos, recordando brevemente o mencionando los tipos que hay (fagocitos, células NK, etc), dado que esto ya se expuso. También se menciona la respuesta inflamatoria y la fiebre, también recordando que ya se expuso. La opción Adquirida tiene las opciones de "natural" o articial", y dentro de cada opción se explican mencionando que depende de los linfocitos de memoria (linfocitos B y T de memoria), y a continiacuión que pueden ser inmunidad activa o pasiva (aplica tanto para natural como adquirida), explicando qué es cada una.</t>
-  </si>
-  <si>
     <t>Responde sobre la inmunización activa y pasiva</t>
   </si>
   <si>
-    <t>Actividad acerca de inmunización activa y pasiva</t>
-  </si>
-  <si>
     <t>Los diferentes tipos de inmunidad</t>
   </si>
   <si>
-    <t>Actividad acerca de la inmunidad natural y adquirida, tanto pasiva como activa</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: El sistema inmunitario</t>
   </si>
   <si>
-    <t>Actividad acerca de la función y los componentes del sistema inmunitario</t>
-  </si>
-  <si>
-    <t>Problemas con el sistema inmunitario</t>
-  </si>
-  <si>
-    <t>Interactivo que explica diversos problemas que pueden darse con y por el sistema inmunitario</t>
-  </si>
-  <si>
     <t>Algunos problemas relacionados con el sistema inmunitario</t>
   </si>
   <si>
-    <t>Actividad acerca de las enfermedades relacionadas con el sistema inmunitario</t>
-  </si>
-  <si>
     <t>El sistema inmunitario y la donación de tejidos</t>
   </si>
   <si>
     <t>Actividad acerca de la respuesta del sistema inmunitario frente a la donación de tejidos</t>
   </si>
   <si>
-    <t>Actividad acerca de las funciones y componentes del sistema inmunitario</t>
-  </si>
-  <si>
     <t>Hacer contenedores, todos sobre inmunidad, usando términos como innata, adquirida natural pasiva, dquirida artificial activa, etc.</t>
   </si>
   <si>
@@ -678,6 +633,66 @@
   </si>
   <si>
     <t>Las enfermedades relacionadas con el sistema inmunitario</t>
+  </si>
+  <si>
+    <t>Interactivo para reconocer diversos problemas que pueden darse con y por el sistema inmunitario</t>
+  </si>
+  <si>
+    <t>Interactivo para entender qué es el sistema inmunitario, el sistema linfático, y reconocer los distintos tipos de glóbulos blancos</t>
+  </si>
+  <si>
+    <t>Menú principal con las opciones "Innata" y "adquirida". La opción Innata no se divide más, y al entrar se habla de que depende de los leucocitos o glóbulos blancos, recordando brevemente o mencionando los tipos que hay (fagocitos, células NK, etc), dado que esto ya se expuso. También se menciona la respuesta inflamatoria y la fiebre, también recordando que ya se expuso. La opción Adquirida tiene las opciones de "natural" o articial", y dentro de cada opción se explican mencionando que depende de los linfocitos de memoria (linfocitos B y T de memoria), y a continiacuión que pueden ser inmunidad activa o pasiva (aplica tanto para natural como adquirida), explicando qué es cada una.</t>
+  </si>
+  <si>
+    <t>Interactivo para reconocer y diferenciar la inmunidad innata y la adquirida</t>
+  </si>
+  <si>
+    <t>Interactivo para comprender y diferenciar las defensas internas y externas de los organismos ante los patógenos</t>
+  </si>
+  <si>
+    <t>Animación para reconocer la estructura y función del sistema linfático</t>
+  </si>
+  <si>
+    <t>Interactivo con animación para entender la función de los diferentes glóbulos blancos</t>
+  </si>
+  <si>
+    <t>Actividad para repasar lo aprendido acerca del sistema linfático</t>
+  </si>
+  <si>
+    <t>Actividad para reconocer y diferenciar los distintos tipos de glóbulos blancos y sus funciones</t>
+  </si>
+  <si>
+    <t>Actividad para reconocer y clasificar los tipos de inmunidad</t>
+  </si>
+  <si>
+    <t>Actividad para analizar la estructura y función del sistema inmunitario</t>
+  </si>
+  <si>
+    <t>Recurso M101A-04</t>
+  </si>
+  <si>
+    <t>Los problemas con el sistema inmunitario</t>
+  </si>
+  <si>
+    <t>Las enfermedades que afectan el sistema inmunitario</t>
+  </si>
+  <si>
+    <t>La donación de tejidos y la respuesta inmunitaria</t>
+  </si>
+  <si>
+    <t>Actividad para analizar las alteraciones del sistema inmunitario y los problemas que presenta durante la donación de tejidos</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Complicaciones relacionadas con el sistema inmunitario</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La respuesta inmunitaria específica</t>
+  </si>
+  <si>
+    <t>Actividades para analizar diversos aspectos de la respuesta inmunitaria específica</t>
+  </si>
+  <si>
+    <t>Actividad para repasar lo aprendido sobre enfermedades del sistema inmunitario</t>
   </si>
 </sst>
 </file>
@@ -1262,11 +1277,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U290"/>
+  <dimension ref="A1:U291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomLeft" activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,7 +1414,7 @@
       <c r="E3" s="13"/>
       <c r="F3" s="9"/>
       <c r="G3" s="16" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="H3" s="9">
         <v>1</v>
@@ -1408,7 +1423,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>140</v>
+        <v>207</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>20</v>
@@ -1430,16 +1445,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="20" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="S3" s="19" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="T3" s="21" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="U3" s="19" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1469,7 +1484,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>20</v>
@@ -1482,7 +1497,7 @@
         <v>43</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>19</v>
@@ -1497,7 +1512,7 @@
         <v>127</v>
       </c>
       <c r="T4" s="21" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="U4" s="19" t="s">
         <v>129</v>
@@ -1521,7 +1536,7 @@
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="16" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H5" s="9">
         <v>3</v>
@@ -1543,7 +1558,7 @@
         <v>52</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="P5" s="9" t="s">
         <v>19</v>
@@ -1558,7 +1573,7 @@
         <v>127</v>
       </c>
       <c r="T5" s="12" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="U5" s="10" t="s">
         <v>129</v>
@@ -1589,7 +1604,7 @@
         <v>19</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>139</v>
+        <v>204</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>20</v>
@@ -1602,7 +1617,7 @@
       </c>
       <c r="N6" s="8"/>
       <c r="O6" s="9" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>19</v>
@@ -1611,16 +1626,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="S6" s="10" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="U6" s="10" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1637,11 +1652,11 @@
         <v>137</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H7" s="9">
         <v>5</v>
@@ -1650,7 +1665,7 @@
         <v>19</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>142</v>
+        <v>208</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>19</v>
@@ -1665,19 +1680,19 @@
         <v>19</v>
       </c>
       <c r="Q7" s="10" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="S7" s="10" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="T7" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="U7" s="10" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1694,11 +1709,11 @@
         <v>137</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="16" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="H8" s="9">
         <v>6</v>
@@ -1707,7 +1722,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>156</v>
+        <v>210</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>20</v>
@@ -1720,7 +1735,7 @@
         <v>32</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="P8" s="9" t="s">
         <v>20</v>
@@ -1755,11 +1770,11 @@
         <v>137</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H9" s="9">
         <v>7</v>
@@ -1768,7 +1783,7 @@
         <v>19</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>149</v>
+        <v>209</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>19</v>
@@ -1783,19 +1798,19 @@
         <v>19</v>
       </c>
       <c r="Q9" s="10" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="R9" s="11" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="S9" s="10" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="T9" s="12" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="U9" s="10" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1812,11 +1827,11 @@
         <v>137</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="16" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H10" s="9">
         <v>8</v>
@@ -1825,7 +1840,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>151</v>
+        <v>211</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>20</v>
@@ -1838,7 +1853,7 @@
         <v>23</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="P10" s="9" t="s">
         <v>19</v>
@@ -1853,7 +1868,7 @@
         <v>127</v>
       </c>
       <c r="T10" s="12" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="U10" s="10" t="s">
         <v>129</v>
@@ -1873,11 +1888,11 @@
         <v>137</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="16" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H11" s="9">
         <v>9</v>
@@ -1886,7 +1901,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>19</v>
@@ -1901,19 +1916,19 @@
         <v>19</v>
       </c>
       <c r="Q11" s="10" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="R11" s="11" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="S11" s="10" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="T11" s="12" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="U11" s="10" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1930,11 +1945,11 @@
         <v>137</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="16" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="H12" s="9">
         <v>10</v>
@@ -1943,7 +1958,7 @@
         <v>19</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>160</v>
+        <v>206</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>20</v>
@@ -1956,7 +1971,7 @@
       </c>
       <c r="N12" s="8"/>
       <c r="O12" s="9" t="s">
-        <v>161</v>
+        <v>205</v>
       </c>
       <c r="P12" s="9" t="s">
         <v>19</v>
@@ -1965,16 +1980,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="11" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="S12" s="10" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="T12" s="12" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="U12" s="10" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1991,13 +2006,13 @@
         <v>137</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="H13" s="9">
         <v>11</v>
@@ -2006,7 +2021,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>165</v>
+        <v>212</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>20</v>
@@ -2019,7 +2034,7 @@
         <v>43</v>
       </c>
       <c r="O13" s="9" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="P13" s="9" t="s">
         <v>19</v>
@@ -2034,7 +2049,7 @@
         <v>127</v>
       </c>
       <c r="T13" s="12" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="U13" s="10" t="s">
         <v>129</v>
@@ -2054,13 +2069,13 @@
         <v>137</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="H14" s="9">
         <v>12</v>
@@ -2069,7 +2084,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>19</v>
@@ -2084,19 +2099,19 @@
         <v>20</v>
       </c>
       <c r="Q14" s="10" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="R14" s="11" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="S14" s="10" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="T14" s="12" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="U14" s="10" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2117,7 +2132,7 @@
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="16" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="H15" s="9">
         <v>13</v>
@@ -2126,7 +2141,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>167</v>
+        <v>213</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>20</v>
@@ -2152,7 +2167,7 @@
         <v>127</v>
       </c>
       <c r="T15" s="12" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="U15" s="10" t="s">
         <v>129</v>
@@ -2169,35 +2184,35 @@
         <v>132</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="E16" s="13"/>
+        <v>137</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>122</v>
+      </c>
       <c r="F16" s="9"/>
       <c r="G16" s="16" t="s">
-        <v>170</v>
+        <v>220</v>
       </c>
       <c r="H16" s="9">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>169</v>
+        <v>221</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>20</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M16" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="N16" s="8"/>
-      <c r="O16" s="9" t="s">
-        <v>212</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="O16" s="9"/>
       <c r="P16" s="9" t="s">
         <v>19</v>
       </c>
@@ -2205,16 +2220,16 @@
         <v>6</v>
       </c>
       <c r="R16" s="11" t="s">
-        <v>198</v>
+        <v>126</v>
       </c>
       <c r="S16" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="T16" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="T16" s="12" t="s">
-        <v>204</v>
-      </c>
       <c r="U16" s="10" t="s">
-        <v>201</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2227,33 +2242,35 @@
       <c r="C17" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="D17" s="15"/>
+      <c r="D17" s="15" t="s">
+        <v>215</v>
+      </c>
       <c r="E17" s="13"/>
       <c r="F17" s="9"/>
       <c r="G17" s="16" t="s">
-        <v>217</v>
+        <v>157</v>
       </c>
       <c r="H17" s="9">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>171</v>
+        <v>203</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>20</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8" t="s">
-        <v>120</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="N17" s="8"/>
       <c r="O17" s="9" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="P17" s="9" t="s">
         <v>19</v>
@@ -2262,16 +2279,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="11" t="s">
-        <v>126</v>
+        <v>183</v>
       </c>
       <c r="S17" s="10" t="s">
-        <v>127</v>
+        <v>184</v>
       </c>
       <c r="T17" s="12" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="U17" s="10" t="s">
-        <v>129</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2284,20 +2301,24 @@
       <c r="C18" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="13"/>
+      <c r="D18" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>216</v>
+      </c>
       <c r="F18" s="9"/>
       <c r="G18" s="16" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="H18" s="9">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>173</v>
+        <v>222</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>20</v>
@@ -2307,10 +2328,10 @@
       </c>
       <c r="M18" s="8"/>
       <c r="N18" s="8" t="s">
-        <v>28</v>
+        <v>120</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="P18" s="9" t="s">
         <v>19</v>
@@ -2325,7 +2346,7 @@
         <v>127</v>
       </c>
       <c r="T18" s="12" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="U18" s="10" t="s">
         <v>129</v>
@@ -2341,22 +2362,24 @@
       <c r="C19" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="D19" s="15"/>
+      <c r="D19" s="15" t="s">
+        <v>215</v>
+      </c>
       <c r="E19" s="13" t="s">
-        <v>122</v>
+        <v>217</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="16" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="H19" s="9">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>20</v>
@@ -2366,9 +2389,11 @@
       </c>
       <c r="M19" s="8"/>
       <c r="N19" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="O19" s="9"/>
+        <v>28</v>
+      </c>
+      <c r="O19" s="9" t="s">
+        <v>196</v>
+      </c>
       <c r="P19" s="9" t="s">
         <v>19</v>
       </c>
@@ -2382,7 +2407,7 @@
         <v>127</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="U19" s="10" t="s">
         <v>129</v>
@@ -2399,48 +2424,52 @@
         <v>132</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="E20" s="13"/>
+        <v>215</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>122</v>
+      </c>
       <c r="F20" s="9"/>
       <c r="G20" s="16" t="s">
-        <v>176</v>
+        <v>219</v>
       </c>
       <c r="H20" s="9">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>177</v>
+        <v>218</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L20" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
+      <c r="N20" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="O20" s="9"/>
       <c r="P20" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="10" t="s">
-        <v>186</v>
+      <c r="Q20" s="10">
+        <v>6</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>187</v>
+        <v>126</v>
       </c>
       <c r="S20" s="10" t="s">
-        <v>188</v>
+        <v>127</v>
       </c>
       <c r="T20" s="12" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="U20" s="10" t="s">
-        <v>189</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2459,16 +2488,16 @@
       <c r="E21" s="13"/>
       <c r="F21" s="9"/>
       <c r="G21" s="16" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="H21" s="9">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>19</v>
@@ -2483,19 +2512,19 @@
         <v>19</v>
       </c>
       <c r="Q21" s="10" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="R21" s="11" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="S21" s="10" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="T21" s="12" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="U21" s="10" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2514,16 +2543,16 @@
       <c r="E22" s="13"/>
       <c r="F22" s="9"/>
       <c r="G22" s="16" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="H22" s="9">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>19</v>
@@ -2538,19 +2567,19 @@
         <v>19</v>
       </c>
       <c r="Q22" s="10" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="R22" s="11" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="S22" s="10" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="T22" s="12" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="U22" s="10" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2564,27 +2593,27 @@
         <v>132</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E23" s="13"/>
       <c r="F23" s="9"/>
       <c r="G23" s="16" t="s">
-        <v>10</v>
+        <v>163</v>
       </c>
       <c r="H23" s="9">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
@@ -2592,11 +2621,21 @@
       <c r="P23" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="11"/>
-      <c r="S23" s="10"/>
-      <c r="T23" s="12"/>
-      <c r="U23" s="10"/>
+      <c r="Q23" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="R23" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="S23" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="T23" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="U23" s="10" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
@@ -2614,46 +2653,34 @@
       <c r="E24" s="13"/>
       <c r="F24" s="9"/>
       <c r="G24" s="16" t="s">
-        <v>125</v>
+        <v>10</v>
       </c>
       <c r="H24" s="9">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>20</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M24" s="8"/>
-      <c r="N24" s="8" t="s">
-        <v>32</v>
-      </c>
+      <c r="N24" s="8"/>
       <c r="O24" s="9"/>
       <c r="P24" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q24" s="10">
-        <v>6</v>
-      </c>
-      <c r="R24" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="S24" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="T24" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="U24" s="10" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="12"/>
+      <c r="U24" s="10"/>
     </row>
     <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
@@ -2671,16 +2698,16 @@
       <c r="E25" s="13"/>
       <c r="F25" s="9"/>
       <c r="G25" s="16" t="s">
-        <v>185</v>
+        <v>125</v>
       </c>
       <c r="H25" s="9">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="K25" s="7" t="s">
         <v>20</v>
@@ -2690,11 +2717,11 @@
       </c>
       <c r="M25" s="8"/>
       <c r="N25" s="8" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="O25" s="9"/>
       <c r="P25" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q25" s="10">
         <v>6</v>
@@ -2706,36 +2733,70 @@
         <v>127</v>
       </c>
       <c r="T25" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="U25" s="10" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="15"/>
+      <c r="A26" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>124</v>
+      </c>
       <c r="E26" s="13"/>
       <c r="F26" s="9"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="6"/>
+      <c r="G26" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="H26" s="9">
+        <v>24</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L26" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
+      <c r="N26" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="10"/>
-      <c r="R26" s="11"/>
-      <c r="S26" s="10"/>
-      <c r="T26" s="12"/>
-      <c r="U26" s="10"/>
-    </row>
-    <row r="27" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P26" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q26" s="10">
+        <v>6</v>
+      </c>
+      <c r="R26" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="S26" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="T26" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="U26" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="24"/>
       <c r="C27" s="14"/>
@@ -2758,7 +2819,7 @@
       <c r="T27" s="12"/>
       <c r="U27" s="10"/>
     </row>
-    <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="24"/>
       <c r="C28" s="14"/>
@@ -2921,7 +2982,7 @@
     </row>
     <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
-      <c r="B35" s="13"/>
+      <c r="B35" s="24"/>
       <c r="C35" s="14"/>
       <c r="D35" s="15"/>
       <c r="E35" s="13"/>
@@ -3885,7 +3946,29 @@
       <c r="T76" s="12"/>
       <c r="U76" s="10"/>
     </row>
-    <row r="78" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="4"/>
+      <c r="B77" s="13"/>
+      <c r="C77" s="14"/>
+      <c r="D77" s="15"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="9"/>
+      <c r="G77" s="16"/>
+      <c r="H77" s="9"/>
+      <c r="I77" s="5"/>
+      <c r="J77" s="17"/>
+      <c r="K77" s="7"/>
+      <c r="L77" s="6"/>
+      <c r="M77" s="8"/>
+      <c r="N77" s="8"/>
+      <c r="O77" s="9"/>
+      <c r="P77" s="9"/>
+      <c r="Q77" s="10"/>
+      <c r="R77" s="11"/>
+      <c r="S77" s="10"/>
+      <c r="T77" s="12"/>
+      <c r="U77" s="10"/>
+    </row>
     <row r="79" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="80" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="81" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
@@ -3898,192 +3981,192 @@
     <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>93</v>
-      </c>
-    </row>
+    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
     </row>
     <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
     </row>
     <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="129" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="130" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="131" hidden="1" x14ac:dyDescent="0.25"/>
@@ -4246,8 +4329,9 @@
     <row r="288" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="289" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="290" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="291" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:U25">
+  <autoFilter ref="A1:U26">
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
@@ -4281,31 +4365,31 @@
           <x14:formula1>
             <xm:f>DATOS!$E$14:$E$48</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N76</xm:sqref>
+          <xm:sqref>N3:N77</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A76</xm:sqref>
+          <xm:sqref>A3:A77</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$D$1:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K76 I3:I76 P3:P76</xm:sqref>
+          <xm:sqref>P3:P77 I3:I77 K3:K77</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$B$1:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>L3:L76</xm:sqref>
+          <xm:sqref>L3:L77</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$1:$E$13</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M76</xm:sqref>
+          <xm:sqref>M3:M77</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Correcciones mapas y adición solicitudes
De los guiones cn_08_02_co, cn_08_03_co y cn_09_03_co
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion03/Escaleta_CN_08_03_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion03/Escaleta_CN_08_03_CO.xlsx
@@ -503,9 +503,6 @@
     <t>El sistema inmunitario y la donación de tejidos</t>
   </si>
   <si>
-    <t>Actividad acerca de la respuesta del sistema inmunitario frente a la donación de tejidos</t>
-  </si>
-  <si>
     <t>Hacer contenedores, todos sobre inmunidad, usando términos como innata, adquirida natural pasiva, dquirida artificial activa, etc.</t>
   </si>
   <si>
@@ -693,6 +690,9 @@
   </si>
   <si>
     <t>Actividad para repasar lo aprendido sobre enfermedades del sistema inmunitario</t>
+  </si>
+  <si>
+    <t>Actividad para repasar y consolidar lo aprendido acerca del comportamiento del sistema inmunitario frente a la donación de tejidos</t>
   </si>
 </sst>
 </file>
@@ -1281,7 +1281,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O18" sqref="O18"/>
+      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1414,7 +1414,7 @@
       <c r="E3" s="13"/>
       <c r="F3" s="9"/>
       <c r="G3" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H3" s="9">
         <v>1</v>
@@ -1423,7 +1423,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>20</v>
@@ -1445,16 +1445,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="S3" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="S3" s="19" t="s">
+      <c r="T3" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="T3" s="21" t="s">
+      <c r="U3" s="19" t="s">
         <v>185</v>
-      </c>
-      <c r="U3" s="19" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1512,7 +1512,7 @@
         <v>127</v>
       </c>
       <c r="T4" s="21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="U4" s="19" t="s">
         <v>129</v>
@@ -1573,7 +1573,7 @@
         <v>127</v>
       </c>
       <c r="T5" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="U5" s="10" t="s">
         <v>129</v>
@@ -1604,7 +1604,7 @@
         <v>19</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>20</v>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="N6" s="8"/>
       <c r="O6" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>19</v>
@@ -1626,16 +1626,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="S6" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="S6" s="10" t="s">
-        <v>184</v>
-      </c>
       <c r="T6" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="U6" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1665,7 +1665,7 @@
         <v>19</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>19</v>
@@ -1680,19 +1680,19 @@
         <v>19</v>
       </c>
       <c r="Q7" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="R7" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="R7" s="11" t="s">
+      <c r="S7" s="10" t="s">
         <v>172</v>
-      </c>
-      <c r="S7" s="10" t="s">
-        <v>173</v>
       </c>
       <c r="T7" s="12" t="s">
         <v>139</v>
       </c>
       <c r="U7" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1722,7 +1722,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>20</v>
@@ -1735,7 +1735,7 @@
         <v>32</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P8" s="9" t="s">
         <v>20</v>
@@ -1783,7 +1783,7 @@
         <v>19</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>19</v>
@@ -1798,19 +1798,19 @@
         <v>19</v>
       </c>
       <c r="Q9" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="R9" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="R9" s="11" t="s">
+      <c r="S9" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="S9" s="10" t="s">
+      <c r="T9" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="U9" s="10" t="s">
         <v>173</v>
-      </c>
-      <c r="T9" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="U9" s="10" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1840,7 +1840,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>20</v>
@@ -1868,7 +1868,7 @@
         <v>127</v>
       </c>
       <c r="T10" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="U10" s="10" t="s">
         <v>129</v>
@@ -1916,19 +1916,19 @@
         <v>19</v>
       </c>
       <c r="Q11" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="R11" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="R11" s="11" t="s">
+      <c r="S11" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="S11" s="10" t="s">
+      <c r="T11" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="U11" s="10" t="s">
         <v>173</v>
-      </c>
-      <c r="T11" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="U11" s="10" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1958,7 +1958,7 @@
         <v>19</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>20</v>
@@ -1971,7 +1971,7 @@
       </c>
       <c r="N12" s="8"/>
       <c r="O12" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="P12" s="9" t="s">
         <v>19</v>
@@ -1980,16 +1980,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="S12" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="S12" s="10" t="s">
-        <v>184</v>
-      </c>
       <c r="T12" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="U12" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2009,7 +2009,7 @@
         <v>152</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G13" s="16" t="s">
         <v>155</v>
@@ -2021,7 +2021,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>20</v>
@@ -2034,7 +2034,7 @@
         <v>43</v>
       </c>
       <c r="O13" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P13" s="9" t="s">
         <v>19</v>
@@ -2049,7 +2049,7 @@
         <v>127</v>
       </c>
       <c r="T13" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="U13" s="10" t="s">
         <v>129</v>
@@ -2072,7 +2072,7 @@
         <v>152</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G14" s="16" t="s">
         <v>154</v>
@@ -2099,19 +2099,19 @@
         <v>20</v>
       </c>
       <c r="Q14" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="R14" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="R14" s="11" t="s">
+      <c r="S14" s="10" t="s">
         <v>172</v>
-      </c>
-      <c r="S14" s="10" t="s">
-        <v>173</v>
       </c>
       <c r="T14" s="12" t="s">
         <v>154</v>
       </c>
       <c r="U14" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2141,7 +2141,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>20</v>
@@ -2167,7 +2167,7 @@
         <v>127</v>
       </c>
       <c r="T15" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="U15" s="10" t="s">
         <v>129</v>
@@ -2191,7 +2191,7 @@
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H16" s="9">
         <v>14</v>
@@ -2200,7 +2200,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>20</v>
@@ -2226,7 +2226,7 @@
         <v>127</v>
       </c>
       <c r="T16" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="U16" s="10" t="s">
         <v>129</v>
@@ -2243,7 +2243,7 @@
         <v>132</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="9"/>
@@ -2257,7 +2257,7 @@
         <v>19</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>20</v>
@@ -2270,7 +2270,7 @@
       </c>
       <c r="N17" s="8"/>
       <c r="O17" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P17" s="9" t="s">
         <v>19</v>
@@ -2279,16 +2279,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="S17" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="S17" s="10" t="s">
-        <v>184</v>
-      </c>
       <c r="T17" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="U17" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2302,14 +2302,14 @@
         <v>132</v>
       </c>
       <c r="D18" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>215</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>216</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H18" s="9">
         <v>16</v>
@@ -2318,7 +2318,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>20</v>
@@ -2331,7 +2331,7 @@
         <v>120</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="P18" s="9" t="s">
         <v>19</v>
@@ -2346,7 +2346,7 @@
         <v>127</v>
       </c>
       <c r="T18" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="U18" s="10" t="s">
         <v>129</v>
@@ -2363,10 +2363,10 @@
         <v>132</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="16" t="s">
@@ -2379,7 +2379,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>159</v>
+        <v>222</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>20</v>
@@ -2392,7 +2392,7 @@
         <v>28</v>
       </c>
       <c r="O19" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P19" s="9" t="s">
         <v>19</v>
@@ -2407,7 +2407,7 @@
         <v>127</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="U19" s="10" t="s">
         <v>129</v>
@@ -2424,14 +2424,14 @@
         <v>132</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>122</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H20" s="9">
         <v>18</v>
@@ -2440,7 +2440,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>20</v>
@@ -2466,7 +2466,7 @@
         <v>127</v>
       </c>
       <c r="T20" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="U20" s="10" t="s">
         <v>129</v>
@@ -2488,7 +2488,7 @@
       <c r="E21" s="13"/>
       <c r="F21" s="9"/>
       <c r="G21" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H21" s="9">
         <v>19</v>
@@ -2497,7 +2497,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>19</v>
@@ -2512,19 +2512,19 @@
         <v>19</v>
       </c>
       <c r="Q21" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="R21" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="R21" s="11" t="s">
+      <c r="S21" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="S21" s="10" t="s">
+      <c r="T21" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="U21" s="10" t="s">
         <v>173</v>
-      </c>
-      <c r="T21" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="U21" s="10" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2543,7 +2543,7 @@
       <c r="E22" s="13"/>
       <c r="F22" s="9"/>
       <c r="G22" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H22" s="9">
         <v>20</v>
@@ -2552,7 +2552,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>19</v>
@@ -2567,19 +2567,19 @@
         <v>19</v>
       </c>
       <c r="Q22" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="R22" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="R22" s="11" t="s">
+      <c r="S22" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="S22" s="10" t="s">
+      <c r="T22" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="U22" s="10" t="s">
         <v>173</v>
-      </c>
-      <c r="T22" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="U22" s="10" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2598,7 +2598,7 @@
       <c r="E23" s="13"/>
       <c r="F23" s="9"/>
       <c r="G23" s="16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H23" s="9">
         <v>21</v>
@@ -2607,7 +2607,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>19</v>
@@ -2622,19 +2622,19 @@
         <v>19</v>
       </c>
       <c r="Q23" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="R23" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="R23" s="11" t="s">
+      <c r="S23" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="S23" s="10" t="s">
+      <c r="T23" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="U23" s="10" t="s">
         <v>173</v>
-      </c>
-      <c r="T23" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="U23" s="10" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2662,7 +2662,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>20</v>
@@ -2707,7 +2707,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K25" s="7" t="s">
         <v>20</v>
@@ -2755,7 +2755,7 @@
       <c r="E26" s="13"/>
       <c r="F26" s="9"/>
       <c r="G26" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H26" s="9">
         <v>24</v>
@@ -2764,7 +2764,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K26" s="7" t="s">
         <v>20</v>

</xml_diff>